<commit_message>
#1 increase content field length
</commit_message>
<xml_diff>
--- a/Customisations/CT Customisations.xlsx
+++ b/Customisations/CT Customisations.xlsx
@@ -227,7 +227,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -240,6 +240,7 @@
     </font>
     <font>
       <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -249,6 +250,10 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -292,31 +297,26 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -716,25 +716,25 @@
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1718,6 +1718,9 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -1814,76 +1817,76 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="4">
         <v>200.0</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5" t="s">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1892,65 +1895,65 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="4">
         <v>-1.0</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5" t="s">
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1959,65 +1962,65 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5" t="s">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="4">
         <v>10000.0</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5" t="s">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2026,131 +2029,131 @@
       <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5" t="s">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N5" s="6">
-        <v>10000.0</v>
-      </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5" t="s">
+        <v>100000.0</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="T5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="V5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="W5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="4">
         <v>300.0</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5" t="s">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="R6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="T6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="U6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="V6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W6" s="5" t="s">
+      <c r="W6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
     </row>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -3124,6 +3127,27 @@
     <row r="976" ht="15.75" customHeight="1"/>
     <row r="977" ht="15.75" customHeight="1"/>
     <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -6351,6 +6375,7 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -6373,40 +6398,40 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>